<commit_message>
karger debugging for st70
</commit_message>
<xml_diff>
--- a/excel/karger_gr17.xlsx
+++ b/excel/karger_gr17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\studia\praca_dyplomowa\git_magisterka\magisterka\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F5B544-4B8D-4422-8047-B3BB3A9D8D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5BBE32-B0B9-4C0D-A4A1-7CA9D90E56C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A6D875E-0F67-4653-8D10-21F433F1A622}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{7A6D875E-0F67-4653-8D10-21F433F1A622}"/>
   </bookViews>
   <sheets>
     <sheet name="Boruvka step 1" sheetId="1" r:id="rId1"/>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8272D6-92E0-46DF-A61E-1D1AF8F3CB02}">
   <dimension ref="A1:X94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="J88" sqref="J88"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>